<commit_message>
fix: Resolve dynomar page critical error by fixing function call order
  - Move snefuru_get_posts_and_pages_data() and
  snefuru_handle_dynolan_ajax()
    to top of dynolan-page.php before they are called
  - Remove duplicate function definitions from bottom of file
  - Update function call pattern to match working pages
  - Use class method approach with safety checks

  Resolves "critical error" on dynomar admin page caused by functions
  being called before they were defined.
</commit_message>
<xml_diff>
--- a/FileGunBasin/9 August-04 StormBasin/320 SDDX xagio training vids notes/SDDX - Xagio Work Site Building August.xlsx
+++ b/FileGunBasin/9 August-04 StormBasin/320 SDDX xagio training vids notes/SDDX - Xagio Work Site Building August.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylecampbell/Documents/repos/localrepo-snefuru4/FileGunBasin/9 August-04 StormBasin/320 SDDX xagio training vids notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76400901-3D63-1A49-9931-364C48C1D335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B791D580-3A37-DA43-B64E-E58DBB6444A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19300" xr2:uid="{3AEF7841-A523-F24D-B9DD-B4AAE3868D65}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>xagio work</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>https://treeserviceannarbor.com/wp-admin/</t>
+  </si>
+  <si>
+    <t>I have 8 builds to do with xagio before the month ends</t>
   </si>
 </sst>
 </file>
@@ -99,9 +102,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -437,11 +441,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB1702C-B5F0-5643-8EAF-29593B02AB60}">
-  <dimension ref="E1:E8"/>
+  <dimension ref="E1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,16 +457,21 @@
     <row r="1" spans="5:5" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E7" t="s">
+    <row r="11" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E8" t="s">
+    <row r="12" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
debug: Add comprehensive error handling to failing admin pages
  - Add try-catch error handling to admin-page.php (snefuru page)
  - Add try-catch error handling to dynolan-page.php (dynomar page)
  - Include detailed error logging and on-screen debug output
  - Check for missing global objects and method existence
  - Log execution steps to identify specific failure points

  Helps diagnose critical errors on /wp-admin/admin.php?page=snefuru
  and /wp-admin/admin.php?page=dynomar pages while preserving
  functionality of working pages.

  Or the shorter version:
  debug: Add error handling to diagnose snefuru and dynomar page failures

  Wraps problematic admin pages in try-catch blocks with detailed
  logging to identify the specific cause of critical errors.
</commit_message>
<xml_diff>
--- a/FileGunBasin/9 August-04 StormBasin/320 SDDX xagio training vids notes/SDDX - Xagio Work Site Building August.xlsx
+++ b/FileGunBasin/9 August-04 StormBasin/320 SDDX xagio training vids notes/SDDX - Xagio Work Site Building August.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylecampbell/Documents/repos/localrepo-snefuru4/FileGunBasin/9 August-04 StormBasin/320 SDDX xagio training vids notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B791D580-3A37-DA43-B64E-E58DBB6444A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE802D3-D394-2A4A-9E41-53D5639558C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19300" xr2:uid="{3AEF7841-A523-F24D-B9DD-B4AAE3868D65}"/>
   </bookViews>
@@ -445,7 +445,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>